<commit_message>
Modificación de la numeración de los recursos por ajustes en el guión CN_06_03_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/SolicitudGrafica_CN_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/SolicitudGrafica_CN_06_03_CO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" tabRatio="500"/>
@@ -11,7 +11,7 @@
     <sheet name="Ayuda" sheetId="2" r:id="rId2"/>
     <sheet name="Definición técnica de imagenes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="218">
   <si>
     <t>Fecha:</t>
   </si>
@@ -508,9 +508,6 @@
     <t>Los seres vivos</t>
   </si>
   <si>
-    <t>Camilo Ernesto Rodríguez Valencia</t>
-  </si>
-  <si>
     <t>Cuaderno de Estudio</t>
   </si>
   <si>
@@ -553,9 +550,6 @@
     <t>IMG04</t>
   </si>
   <si>
-    <t>https://plus.google.com/photos/104361964935097680722/albums/5893501370326884257/5897166949828505058?banner=pwa&amp;pid=5897166949828505058&amp;oid=104361964935097680722</t>
-  </si>
-  <si>
     <t>Árbol filogenético de la vida, los tres dominios</t>
   </si>
   <si>
@@ -571,9 +565,6 @@
     <t>http://www.visualphotos.com/photo/1x6541878/methanosarcina_mazei_archaea_coloured_sem_b244041.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Methanosarcina </t>
-  </si>
-  <si>
     <t>IMG07</t>
   </si>
   <si>
@@ -628,18 +619,12 @@
     <t>IMG13</t>
   </si>
   <si>
-    <t>http://cmaps.cmappers.net/rid=1KNFR8135-GDBWRT-T1S/PARAMECIO.jpg</t>
-  </si>
-  <si>
     <t>Paramecio</t>
   </si>
   <si>
     <t>IMG14</t>
   </si>
   <si>
-    <t>http://www.pv.fagro.edu.uy/fitopato/FOTO%20GALERIA/Citrus_azul/imagepages/image4.html;  http://static.naukas.com/media/2010/11/levaduras.jpg;  https://www.flickr.com/photos/30993596@N02/5063293976/</t>
-  </si>
-  <si>
     <t>Mohos, levaduras y setas</t>
   </si>
   <si>
@@ -667,27 +652,18 @@
     <t>IMG17</t>
   </si>
   <si>
-    <t>http://www.biodiversidad.gob.mx/especies/gran_familia/plantas/musgos/musgos.html</t>
-  </si>
-  <si>
     <t>Musgos, hepáticas y antoceros</t>
   </si>
   <si>
     <t>IMG18</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/d/d1/SoriDicksonia.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pteridofitas </t>
   </si>
   <si>
     <t>IMG19</t>
   </si>
   <si>
-    <t>53029285;  http://www.telecinco.es/bbtfile/6_20121216Vz7HQ6.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Espermatofitas: gimnospermas y angiospermas </t>
   </si>
   <si>
@@ -706,18 +682,9 @@
     <t>IMG21</t>
   </si>
   <si>
-    <t>http://tec55biologia.wikispaces.com/file/view/fotosintesis.JPG/278169666/fotosintesis.JPG</t>
-  </si>
-  <si>
-    <t>Fotosíntesis en hoja</t>
-  </si>
-  <si>
     <t>IMG22</t>
   </si>
   <si>
-    <t>http://dpsteachers.wikispaces.com/M-T</t>
-  </si>
-  <si>
     <t>Collage de animales</t>
   </si>
   <si>
@@ -728,16 +695,47 @@
   </si>
   <si>
     <t>Tejidos animales</t>
+  </si>
+  <si>
+    <t>Fausto Sáenz Jiménez</t>
+  </si>
+  <si>
+    <t>https://lh5.googleusercontent.com/-eq5pX-_geyU/UdbyGKmzreI/AAAAAAAAEqc/w6_-4BRDMtQ/w958-h560-no/figure_01_11_labeled.jpg</t>
+  </si>
+  <si>
+    <t>Methanosarcina</t>
+  </si>
+  <si>
+    <t>Moho 171014882
+Levaduras 48176035
+Setas 209302096</t>
+  </si>
+  <si>
+    <t>Musgo 88706353
+Hepática 189177146
+Antocero 230136289</t>
+  </si>
+  <si>
+    <t>Las tres imágenes se unen según instrucción: la primera (musgo) a la izquierda; la segunda (hepática) en el centro, y la tercera (antocero) en la derecha.</t>
+  </si>
+  <si>
+    <t>Gimnosperma 53029285 Angiospermas 103170473</t>
+  </si>
+  <si>
+    <t>Fotosintesis</t>
+  </si>
+  <si>
+    <t>Traducir el texto de la imagen en inglés así: Oxygen: Oxígeno, Carbo dioxide: Dióxido de carbono, Sugar: Azucar, Light energy: luz del sol, water: agua, minerals: minerales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1451,7 +1449,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1494,9 +1492,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1638,6 +1633,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="5" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1723,24 +1736,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="5" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -1859,7 +1854,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1872,6 +1867,298 @@
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$20" fmlaRange="$J$4:$J$19" noThreeD="1" sel="4" val="0"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2028825</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Drop Down 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2019300</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1657350</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Drop Down 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>1666875</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1032" name="Drop Down 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1032"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1666875</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="Drop Down 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2066925</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>466725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Drop Down 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2085975</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1724025</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>466725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Drop Down 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>466725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Drop Down 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2195,16 +2482,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
@@ -2222,94 +2508,94 @@
     <col min="14" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="80"/>
-      <c r="F2" s="72" t="s">
+      <c r="D2" s="85"/>
+      <c r="F2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="73"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="81">
+      <c r="C3" s="86">
         <v>6</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="F3" s="74">
-        <v>42080</v>
-      </c>
-      <c r="G3" s="75"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
+      <c r="D3" s="87"/>
+      <c r="F3" s="79">
+        <v>42105</v>
+      </c>
+      <c r="G3" s="80"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5">
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="86" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
+      <c r="G4" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="16.5" thickBot="1">
+    <row r="5" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="83" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" s="84"/>
+      <c r="C5" s="88" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="89"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="45" t="str">
+      <c r="F5" s="44" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
         <v/>
       </c>
-      <c r="G5" s="45"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="69"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="68"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2317,20 +2603,20 @@
       <c r="E6" s="7"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="1"/>
@@ -2340,18 +2626,18 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1">
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="76" t="s">
+      <c r="F8" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="78"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="83"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2360,57 +2646,57 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="26.25" thickBot="1">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="68" t="s">
+      <c r="F9" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="68" t="s">
+      <c r="H9" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="68" t="s">
+      <c r="I9" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" ht="81">
+    <row r="10" spans="1:16" s="12" customFormat="1" ht="81" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>142</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="C10" s="27" t="str">
+        <v>148</v>
+      </c>
+      <c r="C10" s="26" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F10" s="14" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
@@ -2429,26 +2715,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J10" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="K10" s="19"/>
-    </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A11" s="13" t="s">
+      <c r="B11" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="103" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="27" t="str">
+      <c r="C11" s="26" t="str">
         <f t="shared" ref="C11:C74" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F11" s="14" t="str">
         <f t="shared" ref="F11:F74" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
@@ -2466,27 +2752,27 @@
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J11" s="104" t="s">
+      <c r="J11" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:16" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A12" s="73" t="s">
         <v>156</v>
       </c>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:16" s="12" customFormat="1" ht="54">
-      <c r="A12" s="105" t="s">
+      <c r="B12" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="B12" s="105" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" s="27" t="str">
+      <c r="C12" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2504,27 +2790,27 @@
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12" s="104" t="s">
+      <c r="J12" s="72" t="s">
+        <v>158</v>
+      </c>
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="1:16" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="K12" s="19"/>
-    </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" ht="108">
-      <c r="A13" s="105" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" s="105" t="s">
-        <v>161</v>
-      </c>
-      <c r="C13" s="27" t="str">
+      <c r="B13" s="73" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F13" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2542,27 +2828,27 @@
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J13" s="104" t="s">
-        <v>162</v>
+      <c r="J13" s="72" t="s">
+        <v>160</v>
       </c>
       <c r="K13" s="19"/>
     </row>
-    <row r="14" spans="1:16" s="12" customFormat="1">
-      <c r="A14" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" s="13">
-        <v>13643572</v>
-      </c>
-      <c r="C14" s="27" t="str">
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="73" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F14" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2580,27 +2866,27 @@
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J14" s="104" t="s">
-        <v>164</v>
+      <c r="J14" s="72" t="s">
+        <v>211</v>
       </c>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="67.5">
-      <c r="A15" s="105" t="s">
-        <v>165</v>
-      </c>
-      <c r="B15" s="105" t="s">
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="108" x14ac:dyDescent="0.25">
+      <c r="A15" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="C15" s="27" t="str">
+      <c r="C15" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F15" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2618,27 +2904,27 @@
         <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J15" s="106" t="s">
+      <c r="J15" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:16" s="12" customFormat="1" ht="108">
-      <c r="A16" s="105" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" s="105" t="s">
-        <v>169</v>
-      </c>
-      <c r="C16" s="27" t="str">
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="1:16" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" s="73">
+        <v>145028542</v>
+      </c>
+      <c r="C16" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F16" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2656,30 +2942,30 @@
         <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J16" s="107" t="s">
-        <v>170</v>
-      </c>
-      <c r="K16" s="29"/>
-    </row>
-    <row r="17" spans="1:11" s="12" customFormat="1">
-      <c r="A17" s="105" t="s">
+      <c r="J16" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="K16" s="28"/>
+    </row>
+    <row r="17" spans="1:11" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="73" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="B17" s="13">
-        <v>145028542</v>
-      </c>
-      <c r="C17" s="27" t="str">
-        <f t="shared" si="0"/>
+      <c r="C17" s="26" t="str">
+        <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F17" s="14" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE($C$7,"_",$A17,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I17="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_06_03_CO_IMG08_small</v>
       </c>
       <c r="G17" s="14" t="str">
@@ -2687,37 +2973,37 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H17" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(I17&lt;&gt;"",I17&lt;&gt;0),IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE($C$7,"_",$A17,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_06_03_CO_IMG08_zoom</v>
       </c>
       <c r="I17" s="14" t="str">
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J17" s="106" t="s">
+      <c r="J17" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="K17" s="21"/>
-    </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" ht="40.5">
-      <c r="A18" s="105" t="s">
-        <v>173</v>
-      </c>
-      <c r="B18" s="105" t="s">
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" s="12" customFormat="1" ht="81" x14ac:dyDescent="0.25">
+      <c r="A18" s="73" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="73" t="s">
         <v>174</v>
       </c>
-      <c r="C18" s="27" t="str">
-        <f t="shared" si="0"/>
+      <c r="C18" s="26" t="str">
+        <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>155</v>
-      </c>
       <c r="F18" s="14" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),CONCATENATE($C$7,"_",$A18,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I18="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_06_03_CO_IMG09_small</v>
       </c>
       <c r="G18" s="14" t="str">
@@ -2725,37 +3011,37 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H18" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(I18&lt;&gt;"",I18&lt;&gt;0),IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),CONCATENATE($C$7,"_",$A18,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_06_03_CO_IMG09_zoom</v>
       </c>
       <c r="I18" s="14" t="str">
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J18" s="106" t="s">
+      <c r="J18" s="75" t="s">
         <v>175</v>
       </c>
-      <c r="K18" s="21"/>
-    </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="81">
-      <c r="A19" s="105" t="s">
-        <v>176</v>
-      </c>
-      <c r="B19" s="105" t="s">
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+      <c r="A19" s="73" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="73" t="s">
         <v>177</v>
       </c>
-      <c r="C19" s="27" t="str">
-        <f t="shared" si="0"/>
+      <c r="C19" s="26" t="str">
+        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F19" s="14" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE($C$7,"_",$A19,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I19="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_06_03_CO_IMG10_small</v>
       </c>
       <c r="G19" s="14" t="str">
@@ -2763,34 +3049,34 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H19" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(I19&lt;&gt;"",I19&lt;&gt;0),IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE($C$7,"_",$A19,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CN_06_03_CO_IMG10_zoom</v>
       </c>
       <c r="I19" s="14" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J19" s="107" t="s">
+      <c r="J19" s="72" t="s">
         <v>178</v>
       </c>
-      <c r="K19" s="29"/>
-    </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" ht="54">
-      <c r="A20" s="105" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" s="105" t="s">
+      <c r="K19" s="28"/>
+    </row>
+    <row r="20" spans="1:11" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="73" t="s">
+        <v>176</v>
+      </c>
+      <c r="B20" s="73" t="s">
         <v>180</v>
       </c>
-      <c r="C20" s="27" t="str">
+      <c r="C20" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F20" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2808,27 +3094,27 @@
         <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J20" s="104" t="s">
+      <c r="J20" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="K20" s="21"/>
-    </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" ht="40.5">
-      <c r="A21" s="105" t="s">
-        <v>182</v>
-      </c>
-      <c r="B21" s="105" t="s">
-        <v>183</v>
-      </c>
-      <c r="C21" s="27" t="str">
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="73" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="73">
+        <v>92979859</v>
+      </c>
+      <c r="C21" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D21" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F21" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2846,27 +3132,27 @@
         <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J21" s="106" t="s">
-        <v>184</v>
-      </c>
-      <c r="K21" s="21"/>
-    </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" ht="54">
-      <c r="A22" s="105" t="s">
-        <v>185</v>
-      </c>
-      <c r="B22" s="105" t="s">
-        <v>186</v>
-      </c>
-      <c r="C22" s="27" t="str">
+      <c r="J21" s="76" t="s">
+        <v>183</v>
+      </c>
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22" spans="1:11" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="73" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="73" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F22" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2884,27 +3170,29 @@
         <f>IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J22" s="108" t="s">
-        <v>187</v>
-      </c>
-      <c r="K22" s="20"/>
-    </row>
-    <row r="23" spans="1:11" s="12" customFormat="1" ht="135">
-      <c r="A23" s="105" t="s">
+      <c r="J22" s="72" t="s">
+        <v>185</v>
+      </c>
+      <c r="K22" s="72" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A23" s="73" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="73" t="s">
         <v>188</v>
       </c>
-      <c r="B23" s="103" t="s">
-        <v>189</v>
-      </c>
-      <c r="C23" s="27" t="str">
+      <c r="C23" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F23" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2922,29 +3210,27 @@
         <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J23" s="104" t="s">
-        <v>190</v>
-      </c>
-      <c r="K23" s="104" t="s">
+      <c r="J23" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="K23" s="72"/>
+    </row>
+    <row r="24" spans="1:11" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="B24" s="73" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" s="12" customFormat="1" ht="54">
-      <c r="A24" s="105" t="s">
-        <v>192</v>
-      </c>
-      <c r="B24" s="105" t="s">
-        <v>193</v>
-      </c>
-      <c r="C24" s="27" t="str">
+      <c r="C24" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D24" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>155</v>
       </c>
       <c r="F24" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2962,27 +3248,27 @@
         <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J24" s="108" t="s">
-        <v>194</v>
+      <c r="J24" s="76" t="s">
+        <v>192</v>
       </c>
       <c r="K24" s="15"/>
     </row>
-    <row r="25" spans="1:11" s="12" customFormat="1" ht="67.5">
-      <c r="A25" s="105" t="s">
-        <v>195</v>
-      </c>
-      <c r="B25" s="105" t="s">
-        <v>196</v>
-      </c>
-      <c r="C25" s="27" t="str">
+    <row r="25" spans="1:11" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25" s="73" t="s">
+        <v>213</v>
+      </c>
+      <c r="C25" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F25" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3000,27 +3286,29 @@
         <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J25" s="108" t="s">
-        <v>197</v>
-      </c>
-      <c r="K25" s="19"/>
-    </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" ht="54">
-      <c r="A26" s="105" t="s">
-        <v>198</v>
-      </c>
-      <c r="B26" s="105" t="s">
-        <v>199</v>
-      </c>
-      <c r="C26" s="27" t="str">
+      <c r="J25" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="K25" s="72" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="73" t="s">
+        <v>193</v>
+      </c>
+      <c r="B26" s="73">
+        <v>103713041</v>
+      </c>
+      <c r="C26" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F26" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3038,27 +3326,27 @@
         <f>IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J26" s="108" t="s">
-        <v>200</v>
+      <c r="J26" s="72" t="s">
+        <v>196</v>
       </c>
       <c r="K26" s="19"/>
     </row>
-    <row r="27" spans="1:11" s="12" customFormat="1" ht="54">
-      <c r="A27" s="105" t="s">
-        <v>201</v>
-      </c>
-      <c r="B27" s="105" t="s">
-        <v>202</v>
-      </c>
-      <c r="C27" s="27" t="str">
+    <row r="27" spans="1:11" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="73" t="s">
+        <v>195</v>
+      </c>
+      <c r="B27" s="73" t="s">
+        <v>215</v>
+      </c>
+      <c r="C27" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F27" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3076,27 +3364,29 @@
         <f>IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J27" s="104" t="s">
-        <v>203</v>
-      </c>
-      <c r="K27" s="19"/>
-    </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" ht="54">
-      <c r="A28" s="105" t="s">
-        <v>204</v>
-      </c>
-      <c r="B28" s="105" t="s">
-        <v>205</v>
-      </c>
-      <c r="C28" s="27" t="str">
+      <c r="J27" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="K27" s="72" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="73" t="s">
+        <v>197</v>
+      </c>
+      <c r="B28" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="C28" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F28" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3114,29 +3404,27 @@
         <f>IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J28" s="104" t="s">
-        <v>206</v>
-      </c>
-      <c r="K28" s="104" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" ht="40.5">
-      <c r="A29" s="105" t="s">
-        <v>208</v>
-      </c>
-      <c r="B29" s="105" t="s">
-        <v>209</v>
-      </c>
-      <c r="C29" s="27" t="str">
+      <c r="J28" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="K28" s="72"/>
+    </row>
+    <row r="29" spans="1:11" s="12" customFormat="1" ht="81" x14ac:dyDescent="0.25">
+      <c r="A29" s="73" t="s">
+        <v>200</v>
+      </c>
+      <c r="B29" s="73">
+        <v>158144057</v>
+      </c>
+      <c r="C29" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D29" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>155</v>
       </c>
       <c r="F29" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3154,27 +3442,29 @@
         <f>IF(OR(B29&lt;&gt;"",J29&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J29" s="104" t="s">
-        <v>210</v>
-      </c>
-      <c r="K29" s="19"/>
-    </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" ht="54">
-      <c r="A30" s="105" t="s">
-        <v>211</v>
-      </c>
-      <c r="B30" s="105" t="s">
-        <v>212</v>
-      </c>
-      <c r="C30" s="27" t="str">
+      <c r="J29" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="K29" s="72" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="73" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" s="73">
+        <v>116264749</v>
+      </c>
+      <c r="C30" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F30" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3192,27 +3482,27 @@
         <f>IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J30" s="104" t="s">
-        <v>213</v>
+      <c r="J30" s="72" t="s">
+        <v>205</v>
       </c>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" ht="27">
-      <c r="A31" s="105" t="s">
-        <v>214</v>
-      </c>
-      <c r="B31" s="105" t="s">
-        <v>215</v>
-      </c>
-      <c r="C31" s="27" t="str">
+    <row r="31" spans="1:11" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="73" t="s">
+        <v>204</v>
+      </c>
+      <c r="B31" s="73" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F31" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3230,27 +3520,27 @@
         <f>IF(OR(B31&lt;&gt;"",J31&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J31" s="104" t="s">
-        <v>216</v>
+      <c r="J31" s="72" t="s">
+        <v>208</v>
       </c>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" spans="1:11" s="12" customFormat="1" ht="40.5">
-      <c r="A32" s="105" t="s">
-        <v>217</v>
-      </c>
-      <c r="B32" s="105" t="s">
-        <v>218</v>
-      </c>
-      <c r="C32" s="27" t="str">
+    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="73" t="s">
+        <v>206</v>
+      </c>
+      <c r="B32" s="73">
+        <v>13643572</v>
+      </c>
+      <c r="C32" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D32" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>155</v>
       </c>
       <c r="F32" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3268,15 +3558,15 @@
         <f>IF(OR(B32&lt;&gt;"",J32&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J32" s="104" t="s">
-        <v>219</v>
+      <c r="J32" s="72" t="s">
+        <v>162</v>
       </c>
       <c r="K32" s="19"/>
     </row>
-    <row r="33" spans="1:11" s="12" customFormat="1">
-      <c r="A33" s="105"/>
+    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="73"/>
       <c r="B33" s="13"/>
-      <c r="C33" s="27" t="str">
+      <c r="C33" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3301,13 +3591,13 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" spans="1:11" s="12" customFormat="1">
+    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="str">
-        <f t="shared" ref="A20:A83" si="3">IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),CONCATENATE(LEFT(A33,3),IF(MID(A33,4,2)+1&lt;10,CONCATENATE("0",MID(A33,4,2)+1),MID(A33,4,2)+1)),"")</f>
+        <f t="shared" ref="A34:A83" si="3">IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),CONCATENATE(LEFT(A33,3),IF(MID(A33,4,2)+1&lt;10,CONCATENATE("0",MID(A33,4,2)+1),MID(A33,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B34" s="13"/>
-      <c r="C34" s="27" t="str">
+      <c r="C34" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3332,13 +3622,13 @@
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
     </row>
-    <row r="35" spans="1:11" s="12" customFormat="1">
+    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B35" s="13"/>
-      <c r="C35" s="27" t="str">
+      <c r="C35" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3363,13 +3653,13 @@
       <c r="J35" s="14"/>
       <c r="K35" s="15"/>
     </row>
-    <row r="36" spans="1:11" s="12" customFormat="1">
+    <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B36" s="13"/>
-      <c r="C36" s="27" t="str">
+      <c r="C36" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3394,13 +3684,13 @@
       <c r="J36" s="14"/>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" spans="1:11" s="12" customFormat="1">
+    <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B37" s="13"/>
-      <c r="C37" s="27" t="str">
+      <c r="C37" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3422,16 +3712,16 @@
         <f>IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J37" s="22"/>
+      <c r="J37" s="21"/>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" spans="1:11" s="12" customFormat="1">
+    <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B38" s="13"/>
-      <c r="C38" s="27" t="str">
+      <c r="C38" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3453,16 +3743,16 @@
         <f>IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J38" s="23"/>
+      <c r="J38" s="22"/>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" spans="1:11" s="12" customFormat="1">
+    <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B39" s="13"/>
-      <c r="C39" s="27" t="str">
+      <c r="C39" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3487,13 +3777,13 @@
       <c r="J39" s="14"/>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" s="12" customFormat="1">
+    <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="27" t="str">
+      <c r="C40" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3518,13 +3808,13 @@
       <c r="J40" s="14"/>
       <c r="K40" s="15"/>
     </row>
-    <row r="41" spans="1:11" s="12" customFormat="1">
+    <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B41" s="13"/>
-      <c r="C41" s="27" t="str">
+      <c r="C41" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3549,13 +3839,13 @@
       <c r="J41" s="14"/>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" s="12" customFormat="1">
+    <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B42" s="13"/>
-      <c r="C42" s="27" t="str">
+      <c r="C42" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3580,13 +3870,13 @@
       <c r="J42" s="14"/>
       <c r="K42" s="15"/>
     </row>
-    <row r="43" spans="1:11" s="12" customFormat="1">
+    <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B43" s="13"/>
-      <c r="C43" s="27" t="str">
+      <c r="C43" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3611,13 +3901,13 @@
       <c r="J43" s="14"/>
       <c r="K43" s="15"/>
     </row>
-    <row r="44" spans="1:11" s="12" customFormat="1">
+    <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B44" s="13"/>
-      <c r="C44" s="27" t="str">
+      <c r="C44" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3642,13 +3932,13 @@
       <c r="J44" s="14"/>
       <c r="K44" s="15"/>
     </row>
-    <row r="45" spans="1:11" s="12" customFormat="1">
+    <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B45" s="13"/>
-      <c r="C45" s="27" t="str">
+      <c r="C45" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3673,13 +3963,13 @@
       <c r="J45" s="14"/>
       <c r="K45" s="15"/>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1">
+    <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B46" s="13"/>
-      <c r="C46" s="27" t="str">
+      <c r="C46" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3704,13 +3994,13 @@
       <c r="J46" s="14"/>
       <c r="K46" s="15"/>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1">
+    <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B47" s="13"/>
-      <c r="C47" s="27" t="str">
+      <c r="C47" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3735,13 +4025,13 @@
       <c r="J47" s="14"/>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" spans="1:11" s="12" customFormat="1">
+    <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B48" s="13"/>
-      <c r="C48" s="27" t="str">
+      <c r="C48" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3766,13 +4056,13 @@
       <c r="J48" s="14"/>
       <c r="K48" s="15"/>
     </row>
-    <row r="49" spans="1:11" s="12" customFormat="1">
+    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B49" s="13"/>
-      <c r="C49" s="27" t="str">
+      <c r="C49" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3797,13 +4087,13 @@
       <c r="J49" s="14"/>
       <c r="K49" s="15"/>
     </row>
-    <row r="50" spans="1:11" s="12" customFormat="1">
+    <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B50" s="13"/>
-      <c r="C50" s="27" t="str">
+      <c r="C50" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3828,13 +4118,13 @@
       <c r="J50" s="14"/>
       <c r="K50" s="15"/>
     </row>
-    <row r="51" spans="1:11" s="12" customFormat="1">
+    <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B51" s="13"/>
-      <c r="C51" s="27" t="str">
+      <c r="C51" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3859,13 +4149,13 @@
       <c r="J51" s="14"/>
       <c r="K51" s="15"/>
     </row>
-    <row r="52" spans="1:11" s="12" customFormat="1">
+    <row r="52" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B52" s="13"/>
-      <c r="C52" s="27" t="str">
+      <c r="C52" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3890,13 +4180,13 @@
       <c r="J52" s="14"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="53" spans="1:11" s="12" customFormat="1">
+    <row r="53" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B53" s="13"/>
-      <c r="C53" s="27" t="str">
+      <c r="C53" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3921,13 +4211,13 @@
       <c r="J53" s="14"/>
       <c r="K53" s="15"/>
     </row>
-    <row r="54" spans="1:11" s="12" customFormat="1">
+    <row r="54" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B54" s="13"/>
-      <c r="C54" s="27" t="str">
+      <c r="C54" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3952,13 +4242,13 @@
       <c r="J54" s="14"/>
       <c r="K54" s="15"/>
     </row>
-    <row r="55" spans="1:11" s="12" customFormat="1">
+    <row r="55" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B55" s="13"/>
-      <c r="C55" s="27" t="str">
+      <c r="C55" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3983,13 +4273,13 @@
       <c r="J55" s="14"/>
       <c r="K55" s="15"/>
     </row>
-    <row r="56" spans="1:11" s="12" customFormat="1">
+    <row r="56" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B56" s="13"/>
-      <c r="C56" s="27" t="str">
+      <c r="C56" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4014,13 +4304,13 @@
       <c r="J56" s="14"/>
       <c r="K56" s="15"/>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1">
+    <row r="57" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B57" s="13"/>
-      <c r="C57" s="27" t="str">
+      <c r="C57" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4045,13 +4335,13 @@
       <c r="J57" s="14"/>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" spans="1:11" s="12" customFormat="1">
+    <row r="58" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B58" s="13"/>
-      <c r="C58" s="27" t="str">
+      <c r="C58" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4076,13 +4366,13 @@
       <c r="J58" s="14"/>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" spans="1:11" s="12" customFormat="1">
+    <row r="59" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B59" s="13"/>
-      <c r="C59" s="27" t="str">
+      <c r="C59" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4107,13 +4397,13 @@
       <c r="J59" s="14"/>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" spans="1:11" s="12" customFormat="1">
+    <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B60" s="13"/>
-      <c r="C60" s="27" t="str">
+      <c r="C60" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4138,13 +4428,13 @@
       <c r="J60" s="14"/>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" spans="1:11" s="12" customFormat="1">
+    <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B61" s="13"/>
-      <c r="C61" s="27" t="str">
+      <c r="C61" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4169,13 +4459,13 @@
       <c r="J61" s="14"/>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" spans="1:11" s="12" customFormat="1">
+    <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B62" s="13"/>
-      <c r="C62" s="27" t="str">
+      <c r="C62" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4200,13 +4490,13 @@
       <c r="J62" s="14"/>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1">
+    <row r="63" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B63" s="13"/>
-      <c r="C63" s="27" t="str">
+      <c r="C63" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4231,13 +4521,13 @@
       <c r="J63" s="14"/>
       <c r="K63" s="15"/>
     </row>
-    <row r="64" spans="1:11" s="12" customFormat="1">
+    <row r="64" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B64" s="13"/>
-      <c r="C64" s="27" t="str">
+      <c r="C64" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4262,13 +4552,13 @@
       <c r="J64" s="14"/>
       <c r="K64" s="15"/>
     </row>
-    <row r="65" spans="1:11" s="12" customFormat="1">
+    <row r="65" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B65" s="13"/>
-      <c r="C65" s="27" t="str">
+      <c r="C65" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4293,13 +4583,13 @@
       <c r="J65" s="14"/>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" s="12" customFormat="1">
+    <row r="66" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B66" s="13"/>
-      <c r="C66" s="27" t="str">
+      <c r="C66" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4324,13 +4614,13 @@
       <c r="J66" s="14"/>
       <c r="K66" s="15"/>
     </row>
-    <row r="67" spans="1:11" s="12" customFormat="1">
+    <row r="67" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B67" s="13"/>
-      <c r="C67" s="27" t="str">
+      <c r="C67" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4355,13 +4645,13 @@
       <c r="J67" s="14"/>
       <c r="K67" s="15"/>
     </row>
-    <row r="68" spans="1:11" s="12" customFormat="1">
+    <row r="68" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B68" s="13"/>
-      <c r="C68" s="27" t="str">
+      <c r="C68" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4386,13 +4676,13 @@
       <c r="J68" s="14"/>
       <c r="K68" s="15"/>
     </row>
-    <row r="69" spans="1:11" s="12" customFormat="1">
+    <row r="69" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B69" s="13"/>
-      <c r="C69" s="27" t="str">
+      <c r="C69" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4417,13 +4707,13 @@
       <c r="J69" s="14"/>
       <c r="K69" s="15"/>
     </row>
-    <row r="70" spans="1:11" s="12" customFormat="1">
+    <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B70" s="13"/>
-      <c r="C70" s="27" t="str">
+      <c r="C70" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4448,13 +4738,13 @@
       <c r="J70" s="14"/>
       <c r="K70" s="15"/>
     </row>
-    <row r="71" spans="1:11" s="12" customFormat="1">
+    <row r="71" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B71" s="13"/>
-      <c r="C71" s="27" t="str">
+      <c r="C71" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4479,13 +4769,13 @@
       <c r="J71" s="14"/>
       <c r="K71" s="15"/>
     </row>
-    <row r="72" spans="1:11" s="12" customFormat="1">
+    <row r="72" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B72" s="13"/>
-      <c r="C72" s="27" t="str">
+      <c r="C72" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4510,13 +4800,13 @@
       <c r="J72" s="14"/>
       <c r="K72" s="15"/>
     </row>
-    <row r="73" spans="1:11" s="12" customFormat="1">
+    <row r="73" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B73" s="13"/>
-      <c r="C73" s="27" t="str">
+      <c r="C73" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4541,13 +4831,13 @@
       <c r="J73" s="14"/>
       <c r="K73" s="15"/>
     </row>
-    <row r="74" spans="1:11" s="12" customFormat="1">
+    <row r="74" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B74" s="13"/>
-      <c r="C74" s="27" t="str">
+      <c r="C74" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4572,13 +4862,13 @@
       <c r="J74" s="14"/>
       <c r="K74" s="15"/>
     </row>
-    <row r="75" spans="1:11" s="12" customFormat="1">
+    <row r="75" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B75" s="13"/>
-      <c r="C75" s="27" t="str">
+      <c r="C75" s="26" t="str">
         <f t="shared" ref="C75:C108" si="4">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
@@ -4603,13 +4893,13 @@
       <c r="J75" s="14"/>
       <c r="K75" s="15"/>
     </row>
-    <row r="76" spans="1:11" s="12" customFormat="1">
+    <row r="76" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B76" s="13"/>
-      <c r="C76" s="27" t="str">
+      <c r="C76" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4634,13 +4924,13 @@
       <c r="J76" s="14"/>
       <c r="K76" s="15"/>
     </row>
-    <row r="77" spans="1:11" s="12" customFormat="1">
+    <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B77" s="13"/>
-      <c r="C77" s="27" t="str">
+      <c r="C77" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4665,13 +4955,13 @@
       <c r="J77" s="14"/>
       <c r="K77" s="15"/>
     </row>
-    <row r="78" spans="1:11" s="12" customFormat="1">
+    <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B78" s="13"/>
-      <c r="C78" s="27" t="str">
+      <c r="C78" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4696,13 +4986,13 @@
       <c r="J78" s="14"/>
       <c r="K78" s="15"/>
     </row>
-    <row r="79" spans="1:11" s="12" customFormat="1">
+    <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B79" s="13"/>
-      <c r="C79" s="27" t="str">
+      <c r="C79" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4727,13 +5017,13 @@
       <c r="J79" s="14"/>
       <c r="K79" s="15"/>
     </row>
-    <row r="80" spans="1:11" s="12" customFormat="1">
+    <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B80" s="13"/>
-      <c r="C80" s="27" t="str">
+      <c r="C80" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4758,13 +5048,13 @@
       <c r="J80" s="14"/>
       <c r="K80" s="15"/>
     </row>
-    <row r="81" spans="1:11" s="12" customFormat="1">
+    <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B81" s="13"/>
-      <c r="C81" s="27" t="str">
+      <c r="C81" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4789,13 +5079,13 @@
       <c r="J81" s="14"/>
       <c r="K81" s="15"/>
     </row>
-    <row r="82" spans="1:11" s="12" customFormat="1">
+    <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B82" s="13"/>
-      <c r="C82" s="27" t="str">
+      <c r="C82" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4820,13 +5110,13 @@
       <c r="J82" s="14"/>
       <c r="K82" s="15"/>
     </row>
-    <row r="83" spans="1:11" s="12" customFormat="1">
+    <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B83" s="13"/>
-      <c r="C83" s="27" t="str">
+      <c r="C83" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4851,13 +5141,13 @@
       <c r="J83" s="14"/>
       <c r="K83" s="15"/>
     </row>
-    <row r="84" spans="1:11" s="12" customFormat="1">
+    <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="str">
         <f t="shared" ref="A84:A108" si="7">IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),CONCATENATE(LEFT(A83,3),IF(MID(A83,4,2)+1&lt;10,CONCATENATE("0",MID(A83,4,2)+1),MID(A83,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B84" s="13"/>
-      <c r="C84" s="27" t="str">
+      <c r="C84" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4882,13 +5172,13 @@
       <c r="J84" s="14"/>
       <c r="K84" s="15"/>
     </row>
-    <row r="85" spans="1:11" s="12" customFormat="1">
+    <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B85" s="13"/>
-      <c r="C85" s="27" t="str">
+      <c r="C85" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4913,13 +5203,13 @@
       <c r="J85" s="14"/>
       <c r="K85" s="15"/>
     </row>
-    <row r="86" spans="1:11" s="12" customFormat="1">
+    <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B86" s="13"/>
-      <c r="C86" s="27" t="str">
+      <c r="C86" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4944,13 +5234,13 @@
       <c r="J86" s="14"/>
       <c r="K86" s="15"/>
     </row>
-    <row r="87" spans="1:11" s="12" customFormat="1">
+    <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B87" s="13"/>
-      <c r="C87" s="27" t="str">
+      <c r="C87" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -4975,13 +5265,13 @@
       <c r="J87" s="14"/>
       <c r="K87" s="15"/>
     </row>
-    <row r="88" spans="1:11" s="12" customFormat="1">
+    <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B88" s="13"/>
-      <c r="C88" s="27" t="str">
+      <c r="C88" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5006,13 +5296,13 @@
       <c r="J88" s="14"/>
       <c r="K88" s="15"/>
     </row>
-    <row r="89" spans="1:11" s="12" customFormat="1">
+    <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B89" s="13"/>
-      <c r="C89" s="27" t="str">
+      <c r="C89" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5037,13 +5327,13 @@
       <c r="J89" s="14"/>
       <c r="K89" s="15"/>
     </row>
-    <row r="90" spans="1:11" s="12" customFormat="1">
+    <row r="90" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B90" s="13"/>
-      <c r="C90" s="27" t="str">
+      <c r="C90" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5068,13 +5358,13 @@
       <c r="J90" s="14"/>
       <c r="K90" s="15"/>
     </row>
-    <row r="91" spans="1:11" s="12" customFormat="1">
+    <row r="91" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B91" s="13"/>
-      <c r="C91" s="27" t="str">
+      <c r="C91" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5099,13 +5389,13 @@
       <c r="J91" s="14"/>
       <c r="K91" s="15"/>
     </row>
-    <row r="92" spans="1:11" s="12" customFormat="1">
+    <row r="92" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B92" s="13"/>
-      <c r="C92" s="27" t="str">
+      <c r="C92" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5130,13 +5420,13 @@
       <c r="J92" s="14"/>
       <c r="K92" s="15"/>
     </row>
-    <row r="93" spans="1:11" s="12" customFormat="1">
+    <row r="93" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B93" s="13"/>
-      <c r="C93" s="27" t="str">
+      <c r="C93" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5161,13 +5451,13 @@
       <c r="J93" s="14"/>
       <c r="K93" s="15"/>
     </row>
-    <row r="94" spans="1:11" s="12" customFormat="1">
+    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B94" s="13"/>
-      <c r="C94" s="27" t="str">
+      <c r="C94" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5192,13 +5482,13 @@
       <c r="J94" s="14"/>
       <c r="K94" s="15"/>
     </row>
-    <row r="95" spans="1:11" s="12" customFormat="1">
+    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B95" s="13"/>
-      <c r="C95" s="27" t="str">
+      <c r="C95" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5223,13 +5513,13 @@
       <c r="J95" s="14"/>
       <c r="K95" s="15"/>
     </row>
-    <row r="96" spans="1:11" s="12" customFormat="1">
+    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B96" s="13"/>
-      <c r="C96" s="27" t="str">
+      <c r="C96" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5254,13 +5544,13 @@
       <c r="J96" s="14"/>
       <c r="K96" s="15"/>
     </row>
-    <row r="97" spans="1:11" s="12" customFormat="1">
+    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B97" s="13"/>
-      <c r="C97" s="27" t="str">
+      <c r="C97" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5285,13 +5575,13 @@
       <c r="J97" s="14"/>
       <c r="K97" s="15"/>
     </row>
-    <row r="98" spans="1:11" s="12" customFormat="1">
+    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B98" s="13"/>
-      <c r="C98" s="27" t="str">
+      <c r="C98" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5316,13 +5606,13 @@
       <c r="J98" s="14"/>
       <c r="K98" s="15"/>
     </row>
-    <row r="99" spans="1:11" s="12" customFormat="1">
+    <row r="99" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B99" s="13"/>
-      <c r="C99" s="27" t="str">
+      <c r="C99" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5347,13 +5637,13 @@
       <c r="J99" s="14"/>
       <c r="K99" s="15"/>
     </row>
-    <row r="100" spans="1:11" s="12" customFormat="1">
+    <row r="100" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B100" s="13"/>
-      <c r="C100" s="27" t="str">
+      <c r="C100" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5378,13 +5668,13 @@
       <c r="J100" s="14"/>
       <c r="K100" s="15"/>
     </row>
-    <row r="101" spans="1:11" s="12" customFormat="1">
+    <row r="101" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B101" s="13"/>
-      <c r="C101" s="27" t="str">
+      <c r="C101" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5409,13 +5699,13 @@
       <c r="J101" s="14"/>
       <c r="K101" s="15"/>
     </row>
-    <row r="102" spans="1:11" s="12" customFormat="1">
+    <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B102" s="13"/>
-      <c r="C102" s="27" t="str">
+      <c r="C102" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5440,13 +5730,13 @@
       <c r="J102" s="14"/>
       <c r="K102" s="15"/>
     </row>
-    <row r="103" spans="1:11" s="12" customFormat="1">
+    <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B103" s="13"/>
-      <c r="C103" s="27" t="str">
+      <c r="C103" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5471,13 +5761,13 @@
       <c r="J103" s="14"/>
       <c r="K103" s="15"/>
     </row>
-    <row r="104" spans="1:11" s="12" customFormat="1">
+    <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B104" s="13"/>
-      <c r="C104" s="27" t="str">
+      <c r="C104" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5502,13 +5792,13 @@
       <c r="J104" s="14"/>
       <c r="K104" s="15"/>
     </row>
-    <row r="105" spans="1:11" s="12" customFormat="1">
+    <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B105" s="13"/>
-      <c r="C105" s="27" t="str">
+      <c r="C105" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5533,13 +5823,13 @@
       <c r="J105" s="14"/>
       <c r="K105" s="15"/>
     </row>
-    <row r="106" spans="1:11" s="12" customFormat="1">
+    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B106" s="13"/>
-      <c r="C106" s="27" t="str">
+      <c r="C106" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5564,13 +5854,13 @@
       <c r="J106" s="14"/>
       <c r="K106" s="15"/>
     </row>
-    <row r="107" spans="1:11" s="12" customFormat="1">
+    <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B107" s="13"/>
-      <c r="C107" s="27" t="str">
+      <c r="C107" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5595,13 +5885,13 @@
       <c r="J107" s="14"/>
       <c r="K107" s="15"/>
     </row>
-    <row r="108" spans="1:11" s="12" customFormat="1">
+    <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="B108" s="13"/>
-      <c r="C108" s="27" t="str">
+      <c r="C108" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -5675,10 +5965,9 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="B23" r:id="rId2" display="http://www.pv.fagro.edu.uy/fitopato/FOTO%20GALERIA/Citrus_azul/imagepages/image4.html; "/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5688,7 +5977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
@@ -5696,541 +5985,541 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.25" style="30" customWidth="1"/>
-    <col min="2" max="2" width="11" style="30"/>
-    <col min="3" max="3" width="13.875" style="30" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="30" customWidth="1"/>
-    <col min="5" max="7" width="11" style="30"/>
-    <col min="8" max="11" width="11" style="30" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="30"/>
+    <col min="1" max="1" width="72.25" style="29" customWidth="1"/>
+    <col min="2" max="2" width="11" style="29"/>
+    <col min="3" max="3" width="13.875" style="29" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="29" customWidth="1"/>
+    <col min="5" max="7" width="11" style="29"/>
+    <col min="8" max="11" width="11" style="29" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="38" t="s">
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="94"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="90" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="91"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="40"/>
-    </row>
-    <row r="3" spans="1:11" ht="63">
-      <c r="A3" s="41" t="s">
+      <c r="D2" s="96"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="39"/>
+    </row>
+    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="96" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="97"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="40"/>
-      <c r="H3" s="30" t="s">
+      <c r="D3" s="102"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="39"/>
+      <c r="H3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="34" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="30" t="s">
+      <c r="F4" s="39"/>
+      <c r="H4" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="29">
         <v>1</v>
       </c>
-      <c r="K4" s="30">
+      <c r="K4" s="29">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="36" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="99" t="str">
+      <c r="D5" s="104" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="100"/>
-      <c r="F5" s="40"/>
-      <c r="H5" s="30" t="s">
+      <c r="E5" s="105"/>
+      <c r="F5" s="39"/>
+      <c r="H5" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="29">
         <v>2</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="29">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1">
-      <c r="A6" s="38" t="s">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
-      <c r="H6" s="30" t="s">
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="H6" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="29">
         <v>3</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="29">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1">
-      <c r="A7" s="41" t="s">
+    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="70" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="85" t="str">
+      <c r="D7" s="90" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="85"/>
-      <c r="F7" s="86"/>
-      <c r="H7" s="30" t="s">
+      <c r="E7" s="90"/>
+      <c r="F7" s="91"/>
+      <c r="H7" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="29">
         <v>4</v>
       </c>
-      <c r="K7" s="30">
+      <c r="K7" s="29">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
-      <c r="I8" s="30" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
+      <c r="I8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="29">
         <v>5</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25">
-      <c r="A9" s="41" t="s">
+    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
-      <c r="I9" s="30" t="s">
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
+      <c r="I9" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="30">
+      <c r="J9" s="29">
         <v>6</v>
       </c>
-      <c r="K9" s="30">
+      <c r="K9" s="29">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1">
-      <c r="A10" s="42" t="s">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
-      <c r="I10" s="30" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
+      <c r="I10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="30">
+      <c r="J10" s="29">
         <v>7</v>
       </c>
-      <c r="K10" s="30">
+      <c r="K10" s="29">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="I11" s="30" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="30">
+      <c r="J11" s="29">
         <v>8</v>
       </c>
-      <c r="K11" s="30">
+      <c r="K11" s="29">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1">
-      <c r="I12" s="30" t="s">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="30">
+      <c r="J12" s="29">
         <v>9</v>
       </c>
-      <c r="K12" s="30">
+      <c r="K12" s="29">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="87" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="89"/>
-      <c r="I13" s="30" t="s">
+      <c r="B13" s="93"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="94"/>
+      <c r="I13" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="30">
+      <c r="J13" s="29">
         <v>10</v>
       </c>
-      <c r="K13" s="30">
+      <c r="K13" s="29">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A14" s="41"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-      <c r="I14" s="30" t="s">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="40"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="I14" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="30">
+      <c r="J14" s="29">
         <v>11</v>
       </c>
-      <c r="K14" s="30">
+      <c r="K14" s="29">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="38" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="90" t="s">
+      <c r="B15" s="38"/>
+      <c r="C15" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="92"/>
-      <c r="J15" s="30">
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="97"/>
+      <c r="J15" s="29">
         <v>12</v>
       </c>
-      <c r="K15" s="30">
+      <c r="K15" s="29">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1">
-      <c r="A16" s="41" t="s">
+    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="34" t="s">
+      <c r="B16" s="38"/>
+      <c r="C16" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="J16" s="30">
+      <c r="J16" s="29">
         <v>13</v>
       </c>
-      <c r="K16" s="30">
+      <c r="K16" s="29">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A17" s="38" t="s">
+    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="36" t="s">
+      <c r="B17" s="38"/>
+      <c r="C17" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="93" t="str">
+      <c r="D17" s="98" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="94"/>
-      <c r="F17" s="95"/>
-      <c r="J17" s="30">
+      <c r="E17" s="99"/>
+      <c r="F17" s="100"/>
+      <c r="J17" s="29">
         <v>14</v>
       </c>
-      <c r="K17" s="30">
+      <c r="K17" s="29">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="70" t="s">
+      <c r="B18" s="38"/>
+      <c r="C18" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="85" t="str">
+      <c r="D18" s="90" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="85"/>
-      <c r="F18" s="86"/>
-      <c r="J18" s="30">
+      <c r="E18" s="90"/>
+      <c r="F18" s="91"/>
+      <c r="J18" s="29">
         <v>15</v>
       </c>
-      <c r="K18" s="30">
+      <c r="K18" s="29">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="38" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40"/>
-      <c r="H19" s="30">
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="39"/>
+      <c r="H19" s="29">
         <v>3</v>
       </c>
-      <c r="J19" s="30">
+      <c r="J19" s="29">
         <v>16</v>
       </c>
-      <c r="K19" s="30">
+      <c r="K19" s="29">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1">
-      <c r="A20" s="42" t="s">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44"/>
-      <c r="H20" s="30">
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="43"/>
+      <c r="H20" s="29">
         <v>4</v>
       </c>
-      <c r="I20" s="30">
+      <c r="I20" s="29">
         <v>5</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J20" s="29">
         <v>4</v>
       </c>
-      <c r="K20" s="30">
+      <c r="K20" s="29">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="H21" s="30" t="str">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H21" s="29" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
       </c>
-      <c r="I21" s="30" t="str">
+      <c r="I21" s="29" t="str">
         <f>CONCATENATE(IF((I20+2)&lt;10,"0",""),I20+2)</f>
         <v>07</v>
       </c>
-      <c r="J21" s="30" t="str">
+      <c r="J21" s="29" t="str">
         <f>CONCATENATE(IF(J20&lt;10,"0",""),J20)</f>
         <v>04</v>
       </c>
-      <c r="K21" s="30">
+      <c r="K21" s="29">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="K22" s="30">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="29">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
-      <c r="K23" s="30">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="29">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="K24" s="30">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="29">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
-      <c r="K25" s="30">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="29">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
-      <c r="K26" s="30">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="29">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
-      <c r="K27" s="30">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="29">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
-      <c r="K28" s="30">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="29">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
-      <c r="K29" s="30">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="29">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
-      <c r="K30" s="30">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="29">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
-      <c r="K31" s="30">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="29">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
-      <c r="K32" s="30">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="29">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11">
-      <c r="K33" s="30">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="29">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11">
-      <c r="K34" s="30">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="29">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11">
-      <c r="K35" s="30">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="29">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11">
-      <c r="K36" s="30">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="29">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11">
-      <c r="K37" s="30">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="29">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11">
-      <c r="K38" s="30">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="29">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11">
-      <c r="K39" s="30">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="29">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11">
-      <c r="K40" s="30">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="29">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11">
-      <c r="K41" s="30">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="29">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11">
-      <c r="K42" s="30">
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="29">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11">
-      <c r="K43" s="30">
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="29">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11">
-      <c r="K44" s="30">
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="29">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11">
-      <c r="K45" s="30" t="str">
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="29" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
       </c>
@@ -6249,12 +6538,173 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId4" name="Drop Down 6">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2028825</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId5" name="Drop Down 7">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2019300</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1657350</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1032" r:id="rId6" name="Drop Down 8">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>1666875</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1035" r:id="rId7" name="Drop Down 11">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>1666875</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId8" name="Drop Down 2">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>38100</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2066925</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>466725</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId9" name="Drop Down 4">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2085975</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1724025</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>466725</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" r:id="rId10" name="Drop Down 5">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>466725</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -6262,564 +6712,564 @@
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="30" customWidth="1"/>
-    <col min="2" max="2" width="22.25" style="30" customWidth="1"/>
-    <col min="3" max="3" width="17.375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="30"/>
-    <col min="5" max="5" width="11.75" style="30" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="30" customWidth="1"/>
-    <col min="7" max="7" width="11" style="30" customWidth="1"/>
-    <col min="8" max="8" width="24.5" style="30" customWidth="1"/>
-    <col min="9" max="9" width="22.25" style="30" customWidth="1"/>
-    <col min="10" max="10" width="20.75" style="30" customWidth="1"/>
-    <col min="11" max="11" width="44.5" style="30" customWidth="1"/>
-    <col min="12" max="16384" width="10.875" style="30"/>
+    <col min="1" max="1" width="21" style="29" customWidth="1"/>
+    <col min="2" max="2" width="22.25" style="29" customWidth="1"/>
+    <col min="3" max="3" width="17.375" style="29" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="29"/>
+    <col min="5" max="5" width="11.75" style="29" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="29" customWidth="1"/>
+    <col min="7" max="7" width="11" style="29" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="29" customWidth="1"/>
+    <col min="9" max="9" width="22.25" style="29" customWidth="1"/>
+    <col min="10" max="10" width="20.75" style="29" customWidth="1"/>
+    <col min="11" max="11" width="44.5" style="29" customWidth="1"/>
+    <col min="12" max="16384" width="10.875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="101" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="106" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="101" t="s">
+      <c r="C1" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="101" t="s">
+      <c r="F1" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="101" t="s">
+      <c r="G1" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="H1" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="101"/>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="49" t="s">
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="106"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="49" t="s">
+      <c r="I2" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="48" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="51" customFormat="1">
-      <c r="A3" s="50" t="s">
+    <row r="3" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50" t="s">
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-    </row>
-    <row r="4" spans="1:11" s="51" customFormat="1">
-      <c r="A4" s="52" t="s">
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+    </row>
+    <row r="4" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52" t="s">
+      <c r="G4" s="51"/>
+      <c r="H4" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="52" t="s">
+      <c r="I4" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="J4" s="52"/>
-    </row>
-    <row r="5" spans="1:11" s="51" customFormat="1">
-      <c r="A5" s="53" t="s">
+      <c r="J4" s="51"/>
+    </row>
+    <row r="5" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="54"/>
-      <c r="H5" s="52" t="s">
+      <c r="G5" s="53"/>
+      <c r="H5" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="I5" s="52" t="s">
+      <c r="I5" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="J5" s="54"/>
-    </row>
-    <row r="6" spans="1:11" s="51" customFormat="1">
-      <c r="A6" s="52" t="s">
+      <c r="J5" s="53"/>
+    </row>
+    <row r="6" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="52" t="s">
+      <c r="H6" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="I6" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="51" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="51" customFormat="1" ht="25.5">
-      <c r="A7" s="52" t="s">
+    <row r="7" spans="1:11" s="50" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52" t="s">
+      <c r="G7" s="51"/>
+      <c r="H7" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="I7" s="52" t="s">
+      <c r="I7" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="J7" s="52"/>
-    </row>
-    <row r="8" spans="1:11" s="51" customFormat="1" ht="25.5">
-      <c r="A8" s="52" t="s">
+      <c r="J7" s="51"/>
+    </row>
+    <row r="8" spans="1:11" s="50" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52" t="s">
+      <c r="G8" s="51"/>
+      <c r="H8" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="I8" s="52" t="s">
+      <c r="I8" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="J8" s="52"/>
-    </row>
-    <row r="9" spans="1:11" s="51" customFormat="1">
-      <c r="A9" s="52" t="s">
+      <c r="J8" s="51"/>
+    </row>
+    <row r="9" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52" t="s">
+      <c r="G9" s="51"/>
+      <c r="H9" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="I9" s="52" t="s">
+      <c r="I9" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="J9" s="52"/>
-    </row>
-    <row r="10" spans="1:11" s="51" customFormat="1">
-      <c r="A10" s="52" t="s">
+      <c r="J9" s="51"/>
+    </row>
+    <row r="10" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52" t="s">
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="I10" s="52" t="s">
+      <c r="I10" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="J10" s="52"/>
-    </row>
-    <row r="11" spans="1:11" s="51" customFormat="1" ht="25.5">
-      <c r="A11" s="52" t="s">
+      <c r="J10" s="51"/>
+    </row>
+    <row r="11" spans="1:11" s="50" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52" t="s">
+      <c r="G11" s="51"/>
+      <c r="H11" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="I11" s="52" t="s">
+      <c r="I11" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="J11" s="52"/>
-    </row>
-    <row r="12" spans="1:11" s="51" customFormat="1">
-      <c r="A12" s="52" t="s">
+      <c r="J11" s="51"/>
+    </row>
+    <row r="12" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52" t="s">
+      <c r="G12" s="51"/>
+      <c r="H12" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="I12" s="52" t="s">
+      <c r="I12" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="J12" s="52"/>
-    </row>
-    <row r="13" spans="1:11" ht="63">
-      <c r="A13" s="55" t="s">
+      <c r="J12" s="51"/>
+    </row>
+    <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A13" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="56"/>
-      <c r="F13" s="57" t="s">
+      <c r="E13" s="55"/>
+      <c r="F13" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="G13" s="55"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52" t="s">
+      <c r="G13" s="54"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="J13" s="55"/>
-      <c r="K13" s="30" t="s">
+      <c r="J13" s="54"/>
+      <c r="K13" s="29" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="55" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="56"/>
-      <c r="F14" s="57" t="s">
+      <c r="E14" s="55"/>
+      <c r="F14" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="G14" s="55"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52" t="s">
+      <c r="G14" s="54"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="J14" s="55"/>
-    </row>
-    <row r="15" spans="1:11" ht="31.5">
-      <c r="A15" s="55" t="s">
+      <c r="J14" s="54"/>
+    </row>
+    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="55" t="s">
+      <c r="D15" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="55" t="s">
+      <c r="E15" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="52" t="s">
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="30" t="s">
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="29" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="94.5">
-      <c r="A16" s="57" t="s">
+    <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="53" t="s">
+      <c r="B16" s="56"/>
+      <c r="C16" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="57" t="s">
+      <c r="D16" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="56" t="s">
+      <c r="E16" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="F16" s="56" t="s">
+      <c r="F16" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="57" t="s">
+      <c r="G16" s="55"/>
+      <c r="H16" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="I16" s="57" t="s">
+      <c r="I16" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="J16" s="56"/>
-      <c r="K16" s="58" t="s">
+      <c r="J16" s="55"/>
+      <c r="K16" s="57" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.5">
-      <c r="A17" s="52" t="s">
+    <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52" t="s">
+      <c r="B17" s="51"/>
+      <c r="C17" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="52" t="s">
+      <c r="F17" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="59" t="s">
+      <c r="G17" s="51"/>
+      <c r="H17" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="I17" s="59" t="s">
+      <c r="I17" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="J17" s="52"/>
-      <c r="K17" s="60" t="s">
+      <c r="J17" s="51"/>
+      <c r="K17" s="59" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="61" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="60" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="62" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="65" t="s">
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="70" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="66" t="s">
         <v>138</v>
       </c>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="65" t="s">
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-    </row>
-    <row r="24" spans="1:11" ht="31.5">
-      <c r="A24" s="65" t="s">
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+    </row>
+    <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="66" t="s">
         <v>144</v>
       </c>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="65" t="s">
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-    </row>
-    <row r="26" spans="1:11" ht="63">
-      <c r="A26" s="65" t="s">
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+    </row>
+    <row r="26" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A26" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Actualización del guión CN_06_03_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/SolicitudGrafica_CN_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/SolicitudGrafica_CN_06_03_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="216">
   <si>
     <t>Fecha:</t>
   </si>
@@ -529,9 +529,6 @@
     <t>IMG02</t>
   </si>
   <si>
-    <t>http://web.educastur.princast.es/proyectos/formadultos/unidades/los_seres_vivos/ud2/6_3.html</t>
-  </si>
-  <si>
     <t>Horizontal</t>
   </si>
   <si>
@@ -541,9 +538,6 @@
     <t>IMG03</t>
   </si>
   <si>
-    <t>http://www.geonomia.org/dokuwiki/doku.php?id=reproduccion_asexual</t>
-  </si>
-  <si>
     <t>Proceso de gemación y fragmentación en hidra y estrella de mar</t>
   </si>
   <si>
@@ -562,15 +556,9 @@
     <t>IMG06</t>
   </si>
   <si>
-    <t>http://www.visualphotos.com/photo/1x6541878/methanosarcina_mazei_archaea_coloured_sem_b244041.jpg</t>
-  </si>
-  <si>
     <t>IMG07</t>
   </si>
   <si>
-    <t>http://1.bp.blogspot.com/-GOyy14I0vpo/Tn22VseAJ6I/AAAAAAAAAQw/wnaZE5-VcBY/s1600/Fuentes+termales+en+Yellowstone.jpg</t>
-  </si>
-  <si>
     <t>Arqueas en fuentes termales de Yellowstone</t>
   </si>
   <si>
@@ -583,36 +571,24 @@
     <t>IMG09</t>
   </si>
   <si>
-    <t>https://cnho.files.wordpress.com/2010/02/biparticion.jpg</t>
-  </si>
-  <si>
     <t>Fisión binaria o bipartición</t>
   </si>
   <si>
     <t>IMG10</t>
   </si>
   <si>
-    <t>http://ejemplosde.info/wp-content/uploads/2013/09/Ejemplos-de-bacterias-caracter%C3%ADsticas.jpg</t>
-  </si>
-  <si>
     <t>Formas bacterianas</t>
   </si>
   <si>
     <t>IMG11</t>
   </si>
   <si>
-    <t>http://www.estudiaronline.org/blog/wp-content/uploads/2013/08/Biodiesel-algas.jpg</t>
-  </si>
-  <si>
     <t>Alga Volvox</t>
   </si>
   <si>
     <t>IMG12</t>
   </si>
   <si>
-    <t>https://www.msu.edu/course/zol/316/lsppscope.htm</t>
-  </si>
-  <si>
     <t>Protozoo leishmania</t>
   </si>
   <si>
@@ -634,9 +610,6 @@
     <t>IMG15</t>
   </si>
   <si>
-    <t>http://www.diversidadmicrobiana.com/index.php?option=com_content&amp;id=690&amp;Itemid=771</t>
-  </si>
-  <si>
     <t>Estructura de un hongo filamentoso</t>
   </si>
   <si>
@@ -673,9 +646,6 @@
     <t>IMG20</t>
   </si>
   <si>
-    <t>http://www.ecured.cu/images/3/37/Tejodo_Vegetal.jpg</t>
-  </si>
-  <si>
     <t>Tejidos vegetales</t>
   </si>
   <si>
@@ -691,16 +661,10 @@
     <t>IMG23</t>
   </si>
   <si>
-    <t>https://dsmbio.files.wordpress.com/2010/05/clip_image0022.jpg</t>
-  </si>
-  <si>
     <t>Tejidos animales</t>
   </si>
   <si>
     <t>Fausto Sáenz Jiménez</t>
-  </si>
-  <si>
-    <t>https://lh5.googleusercontent.com/-eq5pX-_geyU/UdbyGKmzreI/AAAAAAAAEqc/w6_-4BRDMtQ/w958-h560-no/figure_01_11_labeled.jpg</t>
   </si>
   <si>
     <t>Methanosarcina</t>
@@ -726,6 +690,36 @@
   </si>
   <si>
     <t>Traducir el texto de la imagen en inglés así: Oxygen: Oxígeno, Carbo dioxide: Dióxido de carbono, Sugar: Azucar, Light energy: luz del sol, water: agua, minerals: minerales</t>
+  </si>
+  <si>
+    <t>http://commons.wikimedia.org/wiki/File:Silex_spring_in_yellowstone.jpg</t>
+  </si>
+  <si>
+    <t>Ilustración</t>
+  </si>
+  <si>
+    <t>http://standardsingenomics.org/index.php/sigen/article/view/sigs.2505605/708</t>
+  </si>
+  <si>
+    <t>http://en.wikipedia.org/wiki/Leishmaniasis#/media/File:Leishmania_2009-04-14_smear.JPG</t>
+  </si>
+  <si>
+    <t>Elaborar la ilustración similar a la de este link: http://www.geonomia.org/dokuwiki/doku.php?id=reproduccion_asexual</t>
+  </si>
+  <si>
+    <t>Elaborar ilustración a partir de este link: http://web.educastur.princast.es/proyectos/formadultos/unidades/los_seres_vivos/ud2/6_3.html</t>
+  </si>
+  <si>
+    <t>Elaborar ilustración a partir de este link: https://lh5.googleusercontent.com/-eq5pX-_geyU/UdbyGKmzreI/AAAAAAAAEqc/w6_-4BRDMtQ/w958-h560-no/figure_01_11_labeled.jpg</t>
+  </si>
+  <si>
+    <t>Elaborar ilustración a partir del siguiente link: http://ejemplosde.info/wp-content/uploads/2013/09/Ejemplos-de-bacterias-caracter%C3%ADsticas.jpg</t>
+  </si>
+  <si>
+    <t>Elaborar ilustración a partir del siguiente link: http://www.ecured.cu/images/3/37/Tejodo_Vegetal.jpg</t>
+  </si>
+  <si>
+    <t>Elaborar ilustración a partir del siguiente link: https://dsmbio.files.wordpress.com/2010/05/clip_image0022.jpg</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1443,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1736,6 +1730,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="51" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -2486,7 +2486,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -2581,7 +2581,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="88" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D5" s="89"/>
       <c r="E5" s="5"/>
@@ -2719,22 +2719,20 @@
       </c>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="71" t="s">
-        <v>153</v>
-      </c>
+      <c r="B11" s="71"/>
       <c r="C11" s="26" t="str">
         <f t="shared" ref="C11:C74" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F11" s="14" t="str">
         <f t="shared" ref="F11:F74" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
@@ -2753,26 +2751,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J11" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="K11" s="108" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="73" t="s">
         <v>155</v>
       </c>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:16" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="s">
-        <v>156</v>
-      </c>
-      <c r="B12" s="73" t="s">
-        <v>157</v>
-      </c>
+      <c r="B12" s="73"/>
       <c r="C12" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2791,26 +2789,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J12" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="K12" s="19"/>
+        <v>156</v>
+      </c>
+      <c r="K12" s="72" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A13" s="73" t="s">
-        <v>159</v>
-      </c>
-      <c r="B13" s="73" t="s">
-        <v>210</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="B13" s="73"/>
       <c r="C13" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F13" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2829,16 +2827,18 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J13" s="72" t="s">
-        <v>160</v>
-      </c>
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" spans="1:16" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="K13" s="72" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A14" s="73" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>164</v>
+        <v>159</v>
+      </c>
+      <c r="B14" s="109" t="s">
+        <v>208</v>
       </c>
       <c r="C14" s="26" t="str">
         <f t="shared" si="0"/>
@@ -2848,7 +2848,7 @@
         <v>149</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F14" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2867,16 +2867,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="72" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="108" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A15" s="73" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B15" s="73" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="C15" s="26" t="str">
         <f t="shared" si="0"/>
@@ -2886,7 +2886,7 @@
         <v>149</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F15" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2905,13 +2905,13 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="74" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A16" s="73" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B16" s="73">
         <v>145028542</v>
@@ -2924,7 +2924,7 @@
         <v>149</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F16" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2943,16 +2943,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="74" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="K16" s="28"/>
     </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="73" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" s="73" t="s">
-        <v>171</v>
+        <v>164</v>
+      </c>
+      <c r="B17" s="73">
+        <v>255208717</v>
       </c>
       <c r="C17" s="26" t="str">
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -2962,7 +2962,7 @@
         <v>149</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F17" s="14" t="str">
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE($C$7,"_",$A17,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I17="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
@@ -2981,23 +2981,21 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="74" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K17" s="20"/>
     </row>
     <row r="18" spans="1:11" s="12" customFormat="1" ht="81" x14ac:dyDescent="0.25">
       <c r="A18" s="73" t="s">
-        <v>170</v>
-      </c>
-      <c r="B18" s="73" t="s">
-        <v>174</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="B18" s="73"/>
       <c r="C18" s="26" t="str">
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>150</v>
@@ -3019,16 +3017,18 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J18" s="75" t="s">
-        <v>175</v>
-      </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+      <c r="K18" s="74" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A19" s="73" t="s">
-        <v>173</v>
-      </c>
-      <c r="B19" s="73" t="s">
-        <v>177</v>
+        <v>168</v>
+      </c>
+      <c r="B19" s="73">
+        <v>101601940</v>
       </c>
       <c r="C19" s="26" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -3038,7 +3038,7 @@
         <v>149</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F19" s="14" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE($C$7,"_",$A19,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I19="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
@@ -3057,16 +3057,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J19" s="72" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="K19" s="28"/>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="12" customFormat="1" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A20" s="73" t="s">
-        <v>176</v>
-      </c>
-      <c r="B20" s="73" t="s">
-        <v>180</v>
+        <v>170</v>
+      </c>
+      <c r="B20" s="109" t="s">
+        <v>209</v>
       </c>
       <c r="C20" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3076,7 +3076,7 @@
         <v>149</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F20" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3095,13 +3095,13 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J20" s="74" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="73" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B21" s="73">
         <v>92979859</v>
@@ -3133,16 +3133,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J21" s="76" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="K21" s="20"/>
     </row>
     <row r="22" spans="1:11" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A22" s="73" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B22" s="73" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C22" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3152,7 +3152,7 @@
         <v>149</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F22" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3171,18 +3171,18 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J22" s="72" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="K22" s="72" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="73" t="s">
-        <v>184</v>
-      </c>
-      <c r="B23" s="73" t="s">
-        <v>188</v>
+        <v>176</v>
+      </c>
+      <c r="B23" s="73">
+        <v>250764838</v>
       </c>
       <c r="C23" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3192,7 +3192,7 @@
         <v>149</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F23" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3211,16 +3211,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J23" s="76" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="K23" s="72"/>
     </row>
     <row r="24" spans="1:11" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A24" s="73" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B24" s="73" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C24" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3249,16 +3249,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J24" s="76" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="K24" s="15"/>
     </row>
     <row r="25" spans="1:11" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A25" s="73" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B25" s="73" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C25" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3268,7 +3268,7 @@
         <v>149</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F25" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3287,15 +3287,15 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="76" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="K25" s="72" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="73" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B26" s="73">
         <v>103713041</v>
@@ -3308,7 +3308,7 @@
         <v>149</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F26" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3327,16 +3327,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J26" s="72" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="73" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C27" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3346,7 +3346,7 @@
         <v>149</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F27" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3365,28 +3365,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J27" s="72" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="K27" s="72" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
       <c r="A28" s="73" t="s">
-        <v>197</v>
-      </c>
-      <c r="B28" s="73" t="s">
-        <v>201</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="B28" s="73"/>
       <c r="C28" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F28" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3405,13 +3403,15 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J28" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="K28" s="72"/>
+        <v>192</v>
+      </c>
+      <c r="K28" s="72" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="29" spans="1:11" s="12" customFormat="1" ht="81" x14ac:dyDescent="0.25">
       <c r="A29" s="73" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B29" s="73">
         <v>158144057</v>
@@ -3443,15 +3443,15 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J29" s="72" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="K29" s="72" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="73" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B30" s="73">
         <v>116264749</v>
@@ -3464,7 +3464,7 @@
         <v>149</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F30" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3483,26 +3483,24 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J30" s="72" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
       <c r="A31" s="73" t="s">
-        <v>204</v>
-      </c>
-      <c r="B31" s="73" t="s">
-        <v>207</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="B31" s="73"/>
       <c r="C31" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F31" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3521,13 +3519,15 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J31" s="72" t="s">
-        <v>208</v>
-      </c>
-      <c r="K31" s="19"/>
+        <v>197</v>
+      </c>
+      <c r="K31" s="72" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="73" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B32" s="73">
         <v>13643572</v>
@@ -3559,7 +3559,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J32" s="72" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K32" s="19"/>
     </row>
@@ -5964,10 +5964,11 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId1"/>
+    <hyperlink ref="B20" r:id="rId2" location="/media/File:Leishmania_2009-04-14_smear.JPG"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
cambios en imagenes 5, 6, 11 y 15
cambios en imagenes 5, 6, 11 y 15
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/SolicitudGrafica_CN_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/SolicitudGrafica_CN_06_03_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="216">
   <si>
     <t>Fecha:</t>
   </si>
@@ -616,9 +616,6 @@
     <t>IMG16</t>
   </si>
   <si>
-    <t>http://es.wikipedia.org/wiki/Anatom%C3%ADa_de_los_hongos#mediaviewer/File:Amanita_Cesarea_(diagrama).png</t>
-  </si>
-  <si>
     <t>Estructura de una seta</t>
   </si>
   <si>
@@ -692,18 +689,9 @@
     <t>Traducir el texto de la imagen en inglés así: Oxygen: Oxígeno, Carbo dioxide: Dióxido de carbono, Sugar: Azucar, Light energy: luz del sol, water: agua, minerals: minerales</t>
   </si>
   <si>
-    <t>http://commons.wikimedia.org/wiki/File:Silex_spring_in_yellowstone.jpg</t>
-  </si>
-  <si>
     <t>Ilustración</t>
   </si>
   <si>
-    <t>http://standardsingenomics.org/index.php/sigen/article/view/sigs.2505605/708</t>
-  </si>
-  <si>
-    <t>http://en.wikipedia.org/wiki/Leishmaniasis#/media/File:Leishmania_2009-04-14_smear.JPG</t>
-  </si>
-  <si>
     <t>Elaborar la ilustración similar a la de este link: http://www.geonomia.org/dokuwiki/doku.php?id=reproduccion_asexual</t>
   </si>
   <si>
@@ -722,16 +710,16 @@
     <t>Elaborar ilustración a partir del siguiente link: https://dsmbio.files.wordpress.com/2010/05/clip_image0022.jpg</t>
   </si>
   <si>
-    <t>CREDITO : http://standardsingenomics.org/index.php/sigen/article/view/sigs.2505605/708</t>
-  </si>
-  <si>
-    <t>CREDITO: Silex spring in yellowstone by Brocken Inaglory - Own work. Licensed under CC BY-SA 3.0 via Wikimedia Commons - http://commons.wikimedia.org/wiki/File:Silex_spring_in_yellowstone.jpg#/media/File:Silex_spring_in_yellowstone.jpg</t>
-  </si>
-  <si>
-    <t>Credito: "Leishmania 2009-04-14 smear" by Paulo Henrique Orlandi Mourao - Own work. Licensed under CC BY-SA 3.0 via Wikimedia Commons - http://commons.wikimedia.org/wiki/File:Leishmania_2009-04-14_smear.JPG#/media/File:Leishmania_2009-04-14_smear.JPG</t>
-  </si>
-  <si>
-    <t>CREDITO: «Amanita Cesarea (diagrama)» de Arturo D. Castillo (Zoram.hakaan) - Trabajo propio. Disponible bajo la licencia CC BY 3.0 vía Wikimedia Commons - http://commons.wikimedia.org/wiki/File:Amanita_Cesarea_(diagrama).png#/media/File:Amanita_Cesarea_(diagrama).png</t>
+    <t>Ver observaciones</t>
+  </si>
+  <si>
+    <t>Ilustrar según: http://es.wikipedia.org/wiki/Anatom%C3%ADa_de_los_hongos#mediaviewer/File:Amanita_Cesarea_(diagrama).png</t>
+  </si>
+  <si>
+    <t>Ilustrar según muestra:   http://standardsingenomics.org/index.php/sigen/article/view/sigs.2505605/708</t>
+  </si>
+  <si>
+    <t>Ilustrar según  muestra:   http://en.wikipedia.org/wiki/Leishmaniasis#/media/File:Leishmania_2009-04-14_smear.JPG</t>
   </si>
 </sst>
 </file>
@@ -1403,7 +1391,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1478,8 +1466,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1686,7 +1675,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="51" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1773,14 +1762,11 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="72">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1851,6 +1837,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -2547,8 +2534,8 @@
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C20" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2569,7 +2556,7 @@
     <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1">
+    <row r="1" spans="1:16" ht="16" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2581,7 +2568,7 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75">
+    <row r="2" spans="1:16" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>129</v>
@@ -2598,7 +2585,7 @@
       <c r="I2" s="47"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75">
+    <row r="3" spans="1:16" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2615,7 +2602,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5">
+    <row r="4" spans="1:16" ht="15">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
@@ -2636,13 +2623,13 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="16.5" thickBot="1">
+    <row r="5" spans="1:16" ht="16" thickBot="1">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="90" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D5" s="91"/>
       <c r="E5" s="5"/>
@@ -2656,7 +2643,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1">
+    <row r="6" spans="1:16" ht="16" thickBot="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2687,7 +2674,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1">
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="16" thickBot="1">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2707,7 +2694,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="26.25" thickBot="1">
+    <row r="9" spans="1:16" ht="27" thickBot="1">
       <c r="A9" s="27" t="s">
         <v>2</v>
       </c>
@@ -2742,7 +2729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" ht="81">
+    <row r="10" spans="1:16" s="12" customFormat="1" ht="78">
       <c r="A10" s="13" t="s">
         <v>142</v>
       </c>
@@ -2780,7 +2767,7 @@
       </c>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="67.5">
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="65">
       <c r="A11" s="13" t="s">
         <v>152</v>
       </c>
@@ -2790,7 +2777,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>153</v>
@@ -2815,10 +2802,10 @@
         <v>154</v>
       </c>
       <c r="K11" s="77" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="12" customFormat="1" ht="67.5">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="12" customFormat="1" ht="65">
       <c r="A12" s="73" t="s">
         <v>155</v>
       </c>
@@ -2828,7 +2815,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>153</v>
@@ -2853,10 +2840,10 @@
         <v>156</v>
       </c>
       <c r="K12" s="72" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" ht="94.5">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="12" customFormat="1" ht="91">
       <c r="A13" s="73" t="s">
         <v>157</v>
       </c>
@@ -2866,7 +2853,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>153</v>
@@ -2891,22 +2878,22 @@
         <v>158</v>
       </c>
       <c r="K13" s="72" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="12" customFormat="1" ht="90">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="53">
       <c r="A14" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="B14" s="78" t="s">
-        <v>208</v>
+      <c r="B14" t="s">
+        <v>212</v>
       </c>
       <c r="C14" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>149</v>
+        <v>205</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>153</v>
@@ -2928,18 +2915,18 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K14" s="110" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="104">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="26">
       <c r="A15" s="73" t="s">
         <v>161</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>206</v>
+      <c r="B15" s="13">
+        <v>125026373</v>
       </c>
       <c r="C15" s="26" t="str">
         <f t="shared" si="0"/>
@@ -2970,9 +2957,7 @@
       <c r="J15" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="K15" s="110" t="s">
-        <v>217</v>
-      </c>
+      <c r="K15" s="78"/>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1">
       <c r="A16" s="73" t="s">
@@ -3050,7 +3035,7 @@
       </c>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" ht="81">
+    <row r="18" spans="1:11" s="12" customFormat="1" ht="78">
       <c r="A18" s="73" t="s">
         <v>166</v>
       </c>
@@ -3060,7 +3045,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>150</v>
@@ -3085,10 +3070,10 @@
         <v>169</v>
       </c>
       <c r="K18" s="74" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="14.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="12" customFormat="1">
       <c r="A19" s="73" t="s">
         <v>168</v>
       </c>
@@ -3126,12 +3111,12 @@
       </c>
       <c r="K19" s="28"/>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" ht="119">
+    <row r="20" spans="1:11" s="12" customFormat="1" ht="53">
       <c r="A20" s="73" t="s">
         <v>170</v>
       </c>
-      <c r="B20" s="78" t="s">
-        <v>209</v>
+      <c r="B20" t="s">
+        <v>212</v>
       </c>
       <c r="C20" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3163,10 +3148,10 @@
         <v>173</v>
       </c>
       <c r="K20" s="110" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" ht="15">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="12" customFormat="1">
       <c r="A21" s="73" t="s">
         <v>172</v>
       </c>
@@ -3204,12 +3189,12 @@
       </c>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" ht="67.5">
+    <row r="22" spans="1:11" s="12" customFormat="1" ht="65">
       <c r="A22" s="73" t="s">
         <v>174</v>
       </c>
       <c r="B22" s="73" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C22" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3282,19 +3267,19 @@
       </c>
       <c r="K23" s="72"/>
     </row>
-    <row r="24" spans="1:11" s="12" customFormat="1" ht="117">
+    <row r="24" spans="1:11" s="12" customFormat="1" ht="65">
       <c r="A24" s="73" t="s">
         <v>179</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="C24" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>149</v>
+        <v>205</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>150</v>
@@ -3315,11 +3300,11 @@
         <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J24" s="76" t="s">
-        <v>183</v>
-      </c>
-      <c r="K24" s="111" t="s">
-        <v>219</v>
+      <c r="J24" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="12" customFormat="1" ht="65">
@@ -3327,7 +3312,7 @@
         <v>181</v>
       </c>
       <c r="B25" s="73" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C25" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3356,15 +3341,15 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="76" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K25" s="72" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" ht="15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="12" customFormat="1">
       <c r="A26" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B26" s="73">
         <v>103713041</v>
@@ -3396,16 +3381,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J26" s="72" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" s="12" customFormat="1" ht="40.5" customHeight="1">
       <c r="A27" s="73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C27" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3434,15 +3419,15 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J27" s="72" t="s">
+        <v>188</v>
+      </c>
+      <c r="K27" s="72" t="s">
         <v>189</v>
       </c>
-      <c r="K27" s="72" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" ht="54">
+    </row>
+    <row r="28" spans="1:11" s="12" customFormat="1" ht="52">
       <c r="A28" s="73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B28" s="73"/>
       <c r="C28" s="26" t="str">
@@ -3450,7 +3435,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>153</v>
@@ -3472,15 +3457,15 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J28" s="72" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K28" s="72" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" ht="81">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="12" customFormat="1" ht="78">
       <c r="A29" s="73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B29" s="73">
         <v>158144057</v>
@@ -3512,15 +3497,15 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J29" s="72" t="s">
+        <v>203</v>
+      </c>
+      <c r="K29" s="72" t="s">
         <v>204</v>
       </c>
-      <c r="K29" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" ht="15">
+    </row>
+    <row r="30" spans="1:11" s="12" customFormat="1">
       <c r="A30" s="73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B30" s="73">
         <v>116264749</v>
@@ -3552,13 +3537,13 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J30" s="72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" ht="54">
+    <row r="31" spans="1:11" s="12" customFormat="1" ht="52">
       <c r="A31" s="73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B31" s="73"/>
       <c r="C31" s="26" t="str">
@@ -3566,7 +3551,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>153</v>
@@ -3588,15 +3573,15 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J31" s="72" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K31" s="72" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="12" customFormat="1" ht="15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="12" customFormat="1">
       <c r="A32" s="73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B32" s="73">
         <v>13643572</v>
@@ -3660,7 +3645,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="34" spans="1:11" s="12" customFormat="1">
       <c r="A34" s="13" t="str">
         <f t="shared" ref="A34:A83" si="3">IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),CONCATENATE(LEFT(A33,3),IF(MID(A33,4,2)+1&lt;10,CONCATENATE("0",MID(A33,4,2)+1),MID(A33,4,2)+1)),"")</f>
         <v/>
@@ -3691,7 +3676,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
     </row>
-    <row r="35" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="35" spans="1:11" s="12" customFormat="1">
       <c r="A35" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3722,7 +3707,7 @@
       <c r="J35" s="14"/>
       <c r="K35" s="15"/>
     </row>
-    <row r="36" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="36" spans="1:11" s="12" customFormat="1">
       <c r="A36" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3753,7 +3738,7 @@
       <c r="J36" s="14"/>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="37" spans="1:11" s="12" customFormat="1">
       <c r="A37" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3784,7 +3769,7 @@
       <c r="J37" s="21"/>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="38" spans="1:11" s="12" customFormat="1">
       <c r="A38" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3815,7 +3800,7 @@
       <c r="J38" s="22"/>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="39" spans="1:11" s="12" customFormat="1">
       <c r="A39" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3846,7 +3831,7 @@
       <c r="J39" s="14"/>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="40" spans="1:11" s="12" customFormat="1">
       <c r="A40" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3877,7 +3862,7 @@
       <c r="J40" s="14"/>
       <c r="K40" s="15"/>
     </row>
-    <row r="41" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="41" spans="1:11" s="12" customFormat="1">
       <c r="A41" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3908,7 +3893,7 @@
       <c r="J41" s="14"/>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="42" spans="1:11" s="12" customFormat="1">
       <c r="A42" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3939,7 +3924,7 @@
       <c r="J42" s="14"/>
       <c r="K42" s="15"/>
     </row>
-    <row r="43" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="43" spans="1:11" s="12" customFormat="1">
       <c r="A43" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3970,7 +3955,7 @@
       <c r="J43" s="14"/>
       <c r="K43" s="15"/>
     </row>
-    <row r="44" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="44" spans="1:11" s="12" customFormat="1">
       <c r="A44" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4001,7 +3986,7 @@
       <c r="J44" s="14"/>
       <c r="K44" s="15"/>
     </row>
-    <row r="45" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="45" spans="1:11" s="12" customFormat="1">
       <c r="A45" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4032,7 +4017,7 @@
       <c r="J45" s="14"/>
       <c r="K45" s="15"/>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="46" spans="1:11" s="12" customFormat="1">
       <c r="A46" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4063,7 +4048,7 @@
       <c r="J46" s="14"/>
       <c r="K46" s="15"/>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="47" spans="1:11" s="12" customFormat="1">
       <c r="A47" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4094,7 +4079,7 @@
       <c r="J47" s="14"/>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="48" spans="1:11" s="12" customFormat="1">
       <c r="A48" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4125,7 +4110,7 @@
       <c r="J48" s="14"/>
       <c r="K48" s="15"/>
     </row>
-    <row r="49" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="49" spans="1:11" s="12" customFormat="1">
       <c r="A49" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4156,7 +4141,7 @@
       <c r="J49" s="14"/>
       <c r="K49" s="15"/>
     </row>
-    <row r="50" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="50" spans="1:11" s="12" customFormat="1">
       <c r="A50" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4187,7 +4172,7 @@
       <c r="J50" s="14"/>
       <c r="K50" s="15"/>
     </row>
-    <row r="51" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="51" spans="1:11" s="12" customFormat="1">
       <c r="A51" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4218,7 +4203,7 @@
       <c r="J51" s="14"/>
       <c r="K51" s="15"/>
     </row>
-    <row r="52" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="52" spans="1:11" s="12" customFormat="1">
       <c r="A52" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4249,7 +4234,7 @@
       <c r="J52" s="14"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="53" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="53" spans="1:11" s="12" customFormat="1">
       <c r="A53" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4280,7 +4265,7 @@
       <c r="J53" s="14"/>
       <c r="K53" s="15"/>
     </row>
-    <row r="54" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="54" spans="1:11" s="12" customFormat="1">
       <c r="A54" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4311,7 +4296,7 @@
       <c r="J54" s="14"/>
       <c r="K54" s="15"/>
     </row>
-    <row r="55" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="55" spans="1:11" s="12" customFormat="1">
       <c r="A55" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4342,7 +4327,7 @@
       <c r="J55" s="14"/>
       <c r="K55" s="15"/>
     </row>
-    <row r="56" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="56" spans="1:11" s="12" customFormat="1">
       <c r="A56" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4373,7 +4358,7 @@
       <c r="J56" s="14"/>
       <c r="K56" s="15"/>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="57" spans="1:11" s="12" customFormat="1">
       <c r="A57" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4404,7 +4389,7 @@
       <c r="J57" s="14"/>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="58" spans="1:11" s="12" customFormat="1">
       <c r="A58" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4435,7 +4420,7 @@
       <c r="J58" s="14"/>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="59" spans="1:11" s="12" customFormat="1">
       <c r="A59" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4466,7 +4451,7 @@
       <c r="J59" s="14"/>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="60" spans="1:11" s="12" customFormat="1">
       <c r="A60" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4497,7 +4482,7 @@
       <c r="J60" s="14"/>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="61" spans="1:11" s="12" customFormat="1">
       <c r="A61" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4528,7 +4513,7 @@
       <c r="J61" s="14"/>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="62" spans="1:11" s="12" customFormat="1">
       <c r="A62" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4559,7 +4544,7 @@
       <c r="J62" s="14"/>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="63" spans="1:11" s="12" customFormat="1">
       <c r="A63" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4590,7 +4575,7 @@
       <c r="J63" s="14"/>
       <c r="K63" s="15"/>
     </row>
-    <row r="64" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="64" spans="1:11" s="12" customFormat="1">
       <c r="A64" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4621,7 +4606,7 @@
       <c r="J64" s="14"/>
       <c r="K64" s="15"/>
     </row>
-    <row r="65" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="65" spans="1:11" s="12" customFormat="1">
       <c r="A65" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4652,7 +4637,7 @@
       <c r="J65" s="14"/>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="66" spans="1:11" s="12" customFormat="1">
       <c r="A66" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4683,7 +4668,7 @@
       <c r="J66" s="14"/>
       <c r="K66" s="15"/>
     </row>
-    <row r="67" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="67" spans="1:11" s="12" customFormat="1">
       <c r="A67" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4714,7 +4699,7 @@
       <c r="J67" s="14"/>
       <c r="K67" s="15"/>
     </row>
-    <row r="68" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="68" spans="1:11" s="12" customFormat="1">
       <c r="A68" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4745,7 +4730,7 @@
       <c r="J68" s="14"/>
       <c r="K68" s="15"/>
     </row>
-    <row r="69" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="69" spans="1:11" s="12" customFormat="1">
       <c r="A69" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4776,7 +4761,7 @@
       <c r="J69" s="14"/>
       <c r="K69" s="15"/>
     </row>
-    <row r="70" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="70" spans="1:11" s="12" customFormat="1">
       <c r="A70" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4807,7 +4792,7 @@
       <c r="J70" s="14"/>
       <c r="K70" s="15"/>
     </row>
-    <row r="71" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="71" spans="1:11" s="12" customFormat="1">
       <c r="A71" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4838,7 +4823,7 @@
       <c r="J71" s="14"/>
       <c r="K71" s="15"/>
     </row>
-    <row r="72" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="72" spans="1:11" s="12" customFormat="1">
       <c r="A72" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4869,7 +4854,7 @@
       <c r="J72" s="14"/>
       <c r="K72" s="15"/>
     </row>
-    <row r="73" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="73" spans="1:11" s="12" customFormat="1">
       <c r="A73" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4900,7 +4885,7 @@
       <c r="J73" s="14"/>
       <c r="K73" s="15"/>
     </row>
-    <row r="74" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="74" spans="1:11" s="12" customFormat="1">
       <c r="A74" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4931,7 +4916,7 @@
       <c r="J74" s="14"/>
       <c r="K74" s="15"/>
     </row>
-    <row r="75" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="75" spans="1:11" s="12" customFormat="1">
       <c r="A75" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4962,7 +4947,7 @@
       <c r="J75" s="14"/>
       <c r="K75" s="15"/>
     </row>
-    <row r="76" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="76" spans="1:11" s="12" customFormat="1">
       <c r="A76" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4993,7 +4978,7 @@
       <c r="J76" s="14"/>
       <c r="K76" s="15"/>
     </row>
-    <row r="77" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="77" spans="1:11" s="12" customFormat="1">
       <c r="A77" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5024,7 +5009,7 @@
       <c r="J77" s="14"/>
       <c r="K77" s="15"/>
     </row>
-    <row r="78" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="78" spans="1:11" s="12" customFormat="1">
       <c r="A78" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5055,7 +5040,7 @@
       <c r="J78" s="14"/>
       <c r="K78" s="15"/>
     </row>
-    <row r="79" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="79" spans="1:11" s="12" customFormat="1">
       <c r="A79" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5086,7 +5071,7 @@
       <c r="J79" s="14"/>
       <c r="K79" s="15"/>
     </row>
-    <row r="80" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="80" spans="1:11" s="12" customFormat="1">
       <c r="A80" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5117,7 +5102,7 @@
       <c r="J80" s="14"/>
       <c r="K80" s="15"/>
     </row>
-    <row r="81" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="81" spans="1:11" s="12" customFormat="1">
       <c r="A81" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5148,7 +5133,7 @@
       <c r="J81" s="14"/>
       <c r="K81" s="15"/>
     </row>
-    <row r="82" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="82" spans="1:11" s="12" customFormat="1">
       <c r="A82" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5179,7 +5164,7 @@
       <c r="J82" s="14"/>
       <c r="K82" s="15"/>
     </row>
-    <row r="83" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="83" spans="1:11" s="12" customFormat="1">
       <c r="A83" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5210,7 +5195,7 @@
       <c r="J83" s="14"/>
       <c r="K83" s="15"/>
     </row>
-    <row r="84" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="84" spans="1:11" s="12" customFormat="1">
       <c r="A84" s="13" t="str">
         <f t="shared" ref="A84:A108" si="7">IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),CONCATENATE(LEFT(A83,3),IF(MID(A83,4,2)+1&lt;10,CONCATENATE("0",MID(A83,4,2)+1),MID(A83,4,2)+1)),"")</f>
         <v/>
@@ -5241,7 +5226,7 @@
       <c r="J84" s="14"/>
       <c r="K84" s="15"/>
     </row>
-    <row r="85" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="85" spans="1:11" s="12" customFormat="1">
       <c r="A85" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5272,7 +5257,7 @@
       <c r="J85" s="14"/>
       <c r="K85" s="15"/>
     </row>
-    <row r="86" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="86" spans="1:11" s="12" customFormat="1">
       <c r="A86" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5303,7 +5288,7 @@
       <c r="J86" s="14"/>
       <c r="K86" s="15"/>
     </row>
-    <row r="87" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="87" spans="1:11" s="12" customFormat="1">
       <c r="A87" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5334,7 +5319,7 @@
       <c r="J87" s="14"/>
       <c r="K87" s="15"/>
     </row>
-    <row r="88" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="88" spans="1:11" s="12" customFormat="1">
       <c r="A88" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5365,7 +5350,7 @@
       <c r="J88" s="14"/>
       <c r="K88" s="15"/>
     </row>
-    <row r="89" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="89" spans="1:11" s="12" customFormat="1">
       <c r="A89" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5396,7 +5381,7 @@
       <c r="J89" s="14"/>
       <c r="K89" s="15"/>
     </row>
-    <row r="90" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="90" spans="1:11" s="12" customFormat="1">
       <c r="A90" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5427,7 +5412,7 @@
       <c r="J90" s="14"/>
       <c r="K90" s="15"/>
     </row>
-    <row r="91" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="91" spans="1:11" s="12" customFormat="1">
       <c r="A91" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5458,7 +5443,7 @@
       <c r="J91" s="14"/>
       <c r="K91" s="15"/>
     </row>
-    <row r="92" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="92" spans="1:11" s="12" customFormat="1">
       <c r="A92" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5489,7 +5474,7 @@
       <c r="J92" s="14"/>
       <c r="K92" s="15"/>
     </row>
-    <row r="93" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="93" spans="1:11" s="12" customFormat="1">
       <c r="A93" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5520,7 +5505,7 @@
       <c r="J93" s="14"/>
       <c r="K93" s="15"/>
     </row>
-    <row r="94" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="94" spans="1:11" s="12" customFormat="1">
       <c r="A94" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5551,7 +5536,7 @@
       <c r="J94" s="14"/>
       <c r="K94" s="15"/>
     </row>
-    <row r="95" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="95" spans="1:11" s="12" customFormat="1">
       <c r="A95" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5582,7 +5567,7 @@
       <c r="J95" s="14"/>
       <c r="K95" s="15"/>
     </row>
-    <row r="96" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="96" spans="1:11" s="12" customFormat="1">
       <c r="A96" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5613,7 +5598,7 @@
       <c r="J96" s="14"/>
       <c r="K96" s="15"/>
     </row>
-    <row r="97" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="97" spans="1:11" s="12" customFormat="1">
       <c r="A97" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5644,7 +5629,7 @@
       <c r="J97" s="14"/>
       <c r="K97" s="15"/>
     </row>
-    <row r="98" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="98" spans="1:11" s="12" customFormat="1">
       <c r="A98" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5675,7 +5660,7 @@
       <c r="J98" s="14"/>
       <c r="K98" s="15"/>
     </row>
-    <row r="99" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="99" spans="1:11" s="12" customFormat="1">
       <c r="A99" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5706,7 +5691,7 @@
       <c r="J99" s="14"/>
       <c r="K99" s="15"/>
     </row>
-    <row r="100" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="100" spans="1:11" s="12" customFormat="1">
       <c r="A100" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5737,7 +5722,7 @@
       <c r="J100" s="14"/>
       <c r="K100" s="15"/>
     </row>
-    <row r="101" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="101" spans="1:11" s="12" customFormat="1">
       <c r="A101" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5768,7 +5753,7 @@
       <c r="J101" s="14"/>
       <c r="K101" s="15"/>
     </row>
-    <row r="102" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="102" spans="1:11" s="12" customFormat="1">
       <c r="A102" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5799,7 +5784,7 @@
       <c r="J102" s="14"/>
       <c r="K102" s="15"/>
     </row>
-    <row r="103" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="103" spans="1:11" s="12" customFormat="1">
       <c r="A103" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5830,7 +5815,7 @@
       <c r="J103" s="14"/>
       <c r="K103" s="15"/>
     </row>
-    <row r="104" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="104" spans="1:11" s="12" customFormat="1">
       <c r="A104" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5861,7 +5846,7 @@
       <c r="J104" s="14"/>
       <c r="K104" s="15"/>
     </row>
-    <row r="105" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="105" spans="1:11" s="12" customFormat="1">
       <c r="A105" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5892,7 +5877,7 @@
       <c r="J105" s="14"/>
       <c r="K105" s="15"/>
     </row>
-    <row r="106" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="106" spans="1:11" s="12" customFormat="1">
       <c r="A106" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5923,7 +5908,7 @@
       <c r="J106" s="14"/>
       <c r="K106" s="15"/>
     </row>
-    <row r="107" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="107" spans="1:11" s="12" customFormat="1">
       <c r="A107" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5954,7 +5939,7 @@
       <c r="J107" s="14"/>
       <c r="K107" s="15"/>
     </row>
-    <row r="108" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="108" spans="1:11" s="12" customFormat="1">
       <c r="A108" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -6032,10 +6017,6 @@
       <formula1>"3,4,5,6,7,8,9,10,11"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1"/>
-    <hyperlink ref="B20" r:id="rId2" location="/media/File:Leishmania_2009-04-14_smear.JPG"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -6066,7 +6047,7 @@
     <col min="12" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="94" t="s">
         <v>38</v>
       </c>
@@ -6088,7 +6069,7 @@
       <c r="E2" s="99"/>
       <c r="F2" s="39"/>
     </row>
-    <row r="3" spans="1:11" ht="63">
+    <row r="3" spans="1:11" ht="60">
       <c r="A3" s="40" t="s">
         <v>43</v>
       </c>
@@ -6112,7 +6093,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="37" t="s">
         <v>44</v>
       </c>
@@ -6140,7 +6121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1">
+    <row r="5" spans="1:11" ht="76" thickBot="1">
       <c r="A5" s="40" t="s">
         <v>45</v>
       </c>
@@ -6167,7 +6148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1">
+    <row r="6" spans="1:11" ht="31" thickBot="1">
       <c r="A6" s="37" t="s">
         <v>10</v>
       </c>
@@ -6189,7 +6170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1">
+    <row r="7" spans="1:11" ht="46" thickBot="1">
       <c r="A7" s="40" t="s">
         <v>11</v>
       </c>
@@ -6216,7 +6197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25">
+    <row r="8" spans="1:11" ht="45">
       <c r="A8" s="40" t="s">
         <v>53</v>
       </c>
@@ -6235,7 +6216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25">
+    <row r="9" spans="1:11" ht="45">
       <c r="A9" s="40" t="s">
         <v>12</v>
       </c>
@@ -6254,7 +6235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1">
+    <row r="10" spans="1:11" ht="31" thickBot="1">
       <c r="A10" s="41" t="s">
         <v>36</v>
       </c>
@@ -6284,7 +6265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1">
+    <row r="12" spans="1:11" ht="16" thickBot="1">
       <c r="I12" s="29" t="s">
         <v>37</v>
       </c>
@@ -6314,7 +6295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="40"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -6394,7 +6375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1">
+    <row r="18" spans="1:11" ht="76" thickBot="1">
       <c r="A18" s="40" t="s">
         <v>48</v>
       </c>
@@ -6434,7 +6415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1">
+    <row r="20" spans="1:11" ht="61" thickBot="1">
       <c r="A20" s="41" t="s">
         <v>51</v>
       </c>
@@ -6969,7 +6950,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="50" customFormat="1" ht="25.5">
+    <row r="7" spans="1:11" s="50" customFormat="1" ht="28">
       <c r="A7" s="51" t="s">
         <v>80</v>
       </c>
@@ -6997,7 +6978,7 @@
       </c>
       <c r="J7" s="51"/>
     </row>
-    <row r="8" spans="1:11" s="50" customFormat="1" ht="25.5">
+    <row r="8" spans="1:11" s="50" customFormat="1" ht="28">
       <c r="A8" s="51" t="s">
         <v>82</v>
       </c>
@@ -7079,7 +7060,7 @@
       </c>
       <c r="J10" s="51"/>
     </row>
-    <row r="11" spans="1:11" s="50" customFormat="1" ht="25.5">
+    <row r="11" spans="1:11" s="50" customFormat="1" ht="28">
       <c r="A11" s="51" t="s">
         <v>89</v>
       </c>
@@ -7135,7 +7116,7 @@
       </c>
       <c r="J12" s="51"/>
     </row>
-    <row r="13" spans="1:11" ht="63">
+    <row r="13" spans="1:11" ht="60">
       <c r="A13" s="54" t="s">
         <v>93</v>
       </c>
@@ -7186,7 +7167,7 @@
       </c>
       <c r="J14" s="54"/>
     </row>
-    <row r="15" spans="1:11" ht="31.5">
+    <row r="15" spans="1:11" ht="30">
       <c r="A15" s="54" t="s">
         <v>99</v>
       </c>
@@ -7213,7 +7194,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="94.5">
+    <row r="16" spans="1:11" ht="90">
       <c r="A16" s="56" t="s">
         <v>103</v>
       </c>
@@ -7242,7 +7223,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.5">
+    <row r="17" spans="1:11" ht="28">
       <c r="A17" s="51" t="s">
         <v>106</v>
       </c>
@@ -7315,7 +7296,7 @@
       <c r="D23" s="65"/>
       <c r="E23" s="65"/>
     </row>
-    <row r="24" spans="1:11" ht="31.5">
+    <row r="24" spans="1:11" ht="30">
       <c r="A24" s="64" t="s">
         <v>116</v>
       </c>
@@ -7341,7 +7322,7 @@
       <c r="D25" s="65"/>
       <c r="E25" s="65"/>
     </row>
-    <row r="26" spans="1:11" ht="63">
+    <row r="26" spans="1:11" ht="60">
       <c r="A26" s="64" t="s">
         <v>118</v>
       </c>

</xml_diff>